<commit_message>
transferred teacher list who comes
transferred teacher list who comes
</commit_message>
<xml_diff>
--- a/TRE 3 vidhayalaya teacher.xlsx
+++ b/TRE 3 vidhayalaya teacher.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6735"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="11-12" sheetId="1" r:id="rId1"/>
     <sheet name="9-10" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TEACHER LIST_WHO_COMES_ FROM_TR" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Office of DPO (Establishment), Gaya</t>
   </si>
@@ -177,7 +177,31 @@
     <t>nil</t>
   </si>
   <si>
-    <t>grade pay</t>
+    <t>क्रमसं.</t>
+  </si>
+  <si>
+    <t>नाम</t>
+  </si>
+  <si>
+    <t>पदनाम
+BPSC TRE-01/
+BPSC TRE-02/
+EXLUSIVE-01/
+EXLUSIVE-02</t>
+  </si>
+  <si>
+    <t>पदस्थापित विद्यालय का नाम</t>
+  </si>
+  <si>
+    <t>कोटि
+(I-V)/(VI-VIII)
+(IX-X)/(XI-XII)</t>
+  </si>
+  <si>
+    <t>प्राण नंबर</t>
+  </si>
+  <si>
+    <t>अनुभू</t>
   </si>
 </sst>
 </file>
@@ -187,7 +211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +273,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -401,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -457,6 +489,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,7 +801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
@@ -1978,20 +2019,76 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>32</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25">
+        <v>2</v>
+      </c>
+      <c r="C2" s="25">
+        <v>3</v>
+      </c>
+      <c r="D2" s="25">
+        <v>4</v>
+      </c>
+      <c r="E2" s="25">
+        <v>5</v>
+      </c>
+      <c r="F2" s="25">
+        <v>6</v>
+      </c>
+      <c r="G2" s="25">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;8कार्यालय जिला शिक्षा पदाधिकारी, गया
+(स्थापना शाखा)
+जिला में योगदान करने वाले शिक्षकों की सूची</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>